<commit_message>
Atualização automática de TAPERA.xlsx
</commit_message>
<xml_diff>
--- a/TAPERA.xlsx
+++ b/TAPERA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C9BD3D9-46A7-4B27-8F42-0DD72B7689CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{949967D0-1995-4850-A227-582D3B7453C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1284,7 +1284,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{757D2B29-51A0-4880-AA45-F3BF08FD6704}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{40CFD798-7D79-4C40-9C72-FD781152FBCC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1314,10 +1314,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AFF007E-F906-49CF-AE23-B33ADD486169}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435E22FD-1EA8-476E-9D06-8FDD453C9F96}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,7 +1355,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF4B3D03-8788-4CB0-81B5-A42467CD5F1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D9D977-D7A4-49DF-83F9-A925690E4EE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C02214A2-9B15-4A9C-BAFB-65F30F79BD24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{839DD792-476E-419B-BC16-34D11A8AFFA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1437,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8932496E-5927-C0F1-1EC8-5B35B01A56C2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C5977D6-47B1-CC6F-DF51-D1F1961BE281}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1486,7 +1486,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DA01C0C-F8C8-B222-EA86-F895965A7E5D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CB0008C-62AD-8E79-E10C-FF0E119E43D5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1505,7 +1505,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E0CA6A-3686-4234-7291-DEEE53282743}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69567609-90BE-89CB-74A5-291501F78702}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1536,7 +1536,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61DA7FF-0A1C-B3AB-2A8E-33313E0C4BF5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53BDA7B6-DD8A-78D5-187E-E17F203C6639}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1567,7 +1567,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BD02943-721D-C822-0E05-D205479F00E3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B8569D-5E9F-AF57-FD87-0D9757D84C2D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1610,7 +1610,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{665FD7E9-D158-494E-9797-B5D11345DCC9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0877D884-B35A-4931-9869-A7B50F577A66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1648,7 +1648,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{119B3732-434B-4BFC-8F1F-04E4C16B107E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E59AC4F-A734-443A-BD1E-4E5BB14C077C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1691,7 +1691,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B02433-D236-4BA8-B6EB-8A8DD7872DBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F2BC667-2D8D-459A-B567-0E539A869514}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2004,7 +2004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3447D5DE-F859-4766-97AF-714AFDA26FD1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3362C7BB-8492-4F22-AB0B-DA85665319F6}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>